<commit_message>
added Michael's new qval, pval, log2FC .csv files and binarized
</commit_message>
<xml_diff>
--- a/data/other_data/CRISPRi_v1.xlsx
+++ b/data/other_data/CRISPRi_v1.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajinich/Documents/git_repos/mtb_tn_db/data/other_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AD8F9DF9-9D74-4646-9447-49152E041AF8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="10860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRISPRi_phenotypes" sheetId="1" r:id="rId1"/>
@@ -23,7 +29,7 @@
     <sheet name="Rv2182c" sheetId="14" r:id="rId14"/>
     <sheet name="Rv3778c" sheetId="15" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -519,8 +525,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -543,13 +549,33 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFDAC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -583,12 +609,15 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -596,6 +625,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFDAC"/>
+    </mruColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -642,7 +684,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -674,9 +716,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -708,6 +768,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -883,14 +961,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -913,11 +1001,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
@@ -927,7 +1015,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>66</v>
       </c>
@@ -947,11 +1035,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>67</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
@@ -961,7 +1049,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>28</v>
       </c>
@@ -978,16 +1066,17 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>30</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
       </c>
+      <c r="D6" s="4"/>
       <c r="E6" t="s">
         <v>35</v>
       </c>
@@ -995,7 +1084,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>38</v>
       </c>
@@ -1006,7 +1095,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>41</v>
       </c>
@@ -1020,7 +1109,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>42</v>
       </c>
@@ -1031,7 +1120,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>60</v>
       </c>
@@ -1045,7 +1134,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>23</v>
       </c>
@@ -1065,7 +1154,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>31</v>
       </c>
@@ -1082,7 +1171,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>45</v>
       </c>
@@ -1102,7 +1191,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>48</v>
       </c>
@@ -1119,7 +1208,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>20</v>
       </c>
@@ -1138,18 +1227,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -1205,7 +1295,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -1246,7 +1336,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -1281,7 +1371,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>136</v>
       </c>
@@ -1316,7 +1406,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>120</v>
       </c>
@@ -1351,7 +1441,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1388,23 +1478,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -1460,7 +1550,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -1501,7 +1591,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -1542,7 +1632,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>120</v>
       </c>
@@ -1579,22 +1669,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -1650,7 +1740,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -1694,14 +1784,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -1757,7 +1847,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -1795,7 +1885,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -1836,7 +1926,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -1871,7 +1961,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>136</v>
       </c>
@@ -1908,24 +1998,24 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0C00-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0C00-000002000000}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0C00-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -1981,7 +2071,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -2019,7 +2109,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -2060,7 +2150,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -2095,7 +2185,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>136</v>
       </c>
@@ -2130,7 +2220,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>160</v>
       </c>
@@ -2173,25 +2263,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0D00-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0D00-000002000000}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0D00-000003000000}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0D00-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -2247,7 +2337,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -2285,7 +2375,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -2326,7 +2416,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -2361,7 +2451,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>136</v>
       </c>
@@ -2396,7 +2486,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -2433,24 +2523,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0E00-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0E00-000002000000}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0E00-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -2506,7 +2599,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -2547,7 +2640,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -2588,7 +2681,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -2629,7 +2722,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -2670,7 +2763,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -2711,7 +2804,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -2752,7 +2845,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>71</v>
       </c>
@@ -2790,7 +2883,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -2828,7 +2921,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -2863,7 +2956,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>74</v>
       </c>
@@ -2898,7 +2991,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>75</v>
       </c>
@@ -2933,7 +3026,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -2971,7 +3064,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -3011,30 +3104,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
-    <hyperlink ref="D7" r:id="rId6"/>
-    <hyperlink ref="D8" r:id="rId7"/>
-    <hyperlink ref="D9" r:id="rId8"/>
-    <hyperlink ref="D13" r:id="rId9"/>
-    <hyperlink ref="D14" r:id="rId10"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="D13" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="D14" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -3090,7 +3183,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>118</v>
       </c>
@@ -3125,7 +3218,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>119</v>
       </c>
@@ -3163,7 +3256,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>120</v>
       </c>
@@ -3198,7 +3291,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>121</v>
       </c>
@@ -3236,7 +3329,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -3271,7 +3364,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>122</v>
       </c>
@@ -3306,7 +3399,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3341,7 +3434,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>123</v>
       </c>
@@ -3378,23 +3471,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D9" r:id="rId3"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="D9" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -3450,7 +3546,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>118</v>
       </c>
@@ -3485,7 +3581,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>121</v>
       </c>
@@ -3525,21 +3621,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -3595,7 +3691,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -3633,7 +3729,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -3674,7 +3770,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>136</v>
       </c>
@@ -3711,23 +3807,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -3783,7 +3885,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -3821,7 +3923,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -3862,7 +3964,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -3897,7 +3999,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>136</v>
       </c>
@@ -3932,7 +4034,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -3967,7 +4069,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>145</v>
       </c>
@@ -4010,25 +4112,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D7" r:id="rId5"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -4084,7 +4186,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -4125,7 +4227,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>134</v>
       </c>
@@ -4163,7 +4265,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -4204,7 +4306,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>118</v>
       </c>
@@ -4239,7 +4341,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>136</v>
       </c>
@@ -4276,25 +4378,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -4350,7 +4452,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -4385,7 +4487,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -4420,7 +4522,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -4455,7 +4557,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -4495,22 +4597,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1"/>
-    <hyperlink ref="D5" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -4566,7 +4668,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>118</v>
       </c>
@@ -4601,7 +4703,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -4636,7 +4738,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>76</v>
       </c>
@@ -4676,8 +4778,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>